<commit_message>
increased functionality for unit matching
</commit_message>
<xml_diff>
--- a/matched_compositions.xlsx
+++ b/matched_compositions.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,7 +449,15 @@
       <c r="A2" t="inlineStr"/>
       <c r="B2" t="inlineStr">
         <is>
-          <t>clonidine hcl (100mcg) + hydrochlorothiazide (20mg)</t>
+          <t>calcium gluconate (10%w/v) (inj/inf)</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr"/>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>calcium gluconate (10%w/v)</t>
         </is>
       </c>
     </row>

</xml_diff>